<commit_message>
transmit, receive, idle energy model new
</commit_message>
<xml_diff>
--- a/PROPOSAL/Data alive.xlsx
+++ b/PROPOSAL/Data alive.xlsx
@@ -447,1610 +447,1610 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B118" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B122" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B132" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B144" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B145" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B150" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B156" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B158" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B160" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B162" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B163" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B166" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B167" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B172" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B175" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B176" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B177" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B178" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B180" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B181" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B182" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B183" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B184" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B185" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B186" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B192" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B193" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B194" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B195" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B196" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B199" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B200" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B201" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B202" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>